<commit_message>
filled out rubric to this point and fixed some issues where details was located at /details instead of /questions
</commit_message>
<xml_diff>
--- a/Rubric.xlsx
+++ b/Rubric.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
   <si>
     <t>CRITERIA</t>
   </si>
@@ -381,6 +381,9 @@
   </si>
   <si>
     <t>APP</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -907,7 +910,7 @@
   <dimension ref="B1:S64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -988,7 +991,9 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
@@ -999,7 +1004,9 @@
       <c r="C8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1007,7 +1014,9 @@
     <row r="9" spans="2:9" ht="30" customHeight="1">
       <c r="B9" s="11"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1015,7 +1024,9 @@
     <row r="10" spans="2:9" ht="30" customHeight="1">
       <c r="B10" s="11"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1023,7 +1034,9 @@
     <row r="11" spans="2:9" ht="30" customHeight="1">
       <c r="B11" s="11"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1035,7 +1048,9 @@
       <c r="C13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1043,7 +1058,9 @@
     <row r="14" spans="2:9" ht="30" customHeight="1">
       <c r="B14" s="11"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1051,7 +1068,9 @@
     <row r="15" spans="2:9" ht="30" customHeight="1">
       <c r="B15" s="11"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="7"/>
+      <c r="D15" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>16</v>
       </c>
@@ -1059,7 +1078,9 @@
     <row r="16" spans="2:9" ht="30" customHeight="1">
       <c r="B16" s="11"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1067,7 +1088,9 @@
     <row r="17" spans="2:19" ht="30" customHeight="1">
       <c r="B17" s="11"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="7"/>
+      <c r="D17" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>18</v>
       </c>
@@ -1077,7 +1100,9 @@
     <row r="18" spans="2:19" ht="30" customHeight="1">
       <c r="B18" s="11"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="7"/>
+      <c r="D18" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1087,7 +1112,9 @@
       <c r="C19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>21</v>
       </c>
@@ -1095,7 +1122,9 @@
     <row r="20" spans="2:19" ht="30" customHeight="1">
       <c r="B20" s="11"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="7"/>
+      <c r="D20" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1103,7 +1132,9 @@
     <row r="21" spans="2:19" ht="30" customHeight="1">
       <c r="B21" s="11"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="7"/>
+      <c r="D21" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1115,7 +1146,9 @@
       <c r="C22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="7"/>
+      <c r="D22" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1131,7 +1164,9 @@
     <row r="24" spans="2:19" ht="30" customHeight="1">
       <c r="B24" s="11"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="7"/>
+      <c r="D24" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E24" s="10" t="s">
         <v>27</v>
       </c>
@@ -1147,7 +1182,9 @@
     <row r="26" spans="2:19" ht="30" customHeight="1">
       <c r="B26" s="11"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="7"/>
+      <c r="D26" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E26" s="10" t="s">
         <v>29</v>
       </c>
@@ -1155,7 +1192,9 @@
     <row r="27" spans="2:19" ht="30" customHeight="1">
       <c r="B27" s="11"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="7"/>
+      <c r="D27" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E27" s="2" t="s">
         <v>30</v>
       </c>
@@ -1163,7 +1202,9 @@
     <row r="28" spans="2:19" ht="30" customHeight="1">
       <c r="B28" s="11"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="7"/>
+      <c r="D28" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E28" s="10" t="s">
         <v>31</v>
       </c>
@@ -1171,7 +1212,9 @@
     <row r="29" spans="2:19" ht="30" customHeight="1">
       <c r="B29" s="11"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="7"/>
+      <c r="D29" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E29" s="10" t="s">
         <v>32</v>
       </c>
@@ -1179,7 +1222,9 @@
     <row r="30" spans="2:19" ht="30" customHeight="1">
       <c r="B30" s="11"/>
       <c r="C30" s="9"/>
-      <c r="D30" s="7"/>
+      <c r="D30" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E30" s="10" t="s">
         <v>33</v>
       </c>
@@ -1187,7 +1232,9 @@
     <row r="31" spans="2:19" ht="30" customHeight="1">
       <c r="B31" s="11"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="7"/>
+      <c r="D31" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E31" s="2" t="s">
         <v>34</v>
       </c>
@@ -1195,7 +1242,9 @@
     <row r="32" spans="2:19" ht="30" customHeight="1">
       <c r="B32" s="11"/>
       <c r="C32" s="9"/>
-      <c r="D32" s="7"/>
+      <c r="D32" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E32" s="2" t="s">
         <v>35</v>
       </c>
@@ -1203,7 +1252,9 @@
     <row r="33" spans="2:5" ht="30" customHeight="1">
       <c r="B33" s="11"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="7"/>
+      <c r="D33" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1213,7 +1264,9 @@
       <c r="C34" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="7"/>
+      <c r="D34" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1221,7 +1274,9 @@
     <row r="35" spans="2:5" ht="30" customHeight="1">
       <c r="B35" s="11"/>
       <c r="C35" s="9"/>
-      <c r="D35" s="7"/>
+      <c r="D35" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1229,7 +1284,9 @@
     <row r="36" spans="2:5" ht="30" customHeight="1">
       <c r="B36" s="11"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="7"/>
+      <c r="D36" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E36" s="2" t="s">
         <v>40</v>
       </c>
@@ -1249,7 +1306,9 @@
       <c r="C38" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="7"/>
+      <c r="D38" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1257,7 +1316,9 @@
     <row r="39" spans="2:5" ht="30" customHeight="1">
       <c r="B39" s="11"/>
       <c r="C39" s="9"/>
-      <c r="D39" s="7"/>
+      <c r="D39" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1273,7 +1334,9 @@
     <row r="41" spans="2:5" ht="30" customHeight="1">
       <c r="B41" s="11"/>
       <c r="C41" s="9"/>
-      <c r="D41" s="7"/>
+      <c r="D41" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E41" s="2" t="s">
         <v>46</v>
       </c>
@@ -1285,7 +1348,9 @@
       <c r="C42" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D42" s="7"/>
+      <c r="D42" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E42" s="2" t="s">
         <v>48</v>
       </c>
@@ -1345,7 +1410,9 @@
       <c r="C49" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="7"/>
+      <c r="D49" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E49" s="1" t="s">
         <v>56</v>
       </c>
@@ -1353,7 +1420,9 @@
     <row r="50" spans="2:5" ht="30" customHeight="1">
       <c r="B50" s="11"/>
       <c r="C50" s="9"/>
-      <c r="D50" s="7"/>
+      <c r="D50" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E50" s="1" t="s">
         <v>57</v>
       </c>
@@ -1365,7 +1434,9 @@
       <c r="C51" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D51" s="7"/>
+      <c r="D51" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E51" s="1" t="s">
         <v>59</v>
       </c>
@@ -1373,7 +1444,9 @@
     <row r="52" spans="2:5" ht="30" customHeight="1">
       <c r="B52" s="11"/>
       <c r="C52" s="9"/>
-      <c r="D52" s="7"/>
+      <c r="D52" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E52" s="1" t="s">
         <v>60</v>
       </c>
@@ -1395,7 +1468,9 @@
       <c r="C56" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D56" s="7"/>
+      <c r="D56" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E56" s="1" t="s">
         <v>71</v>
       </c>
@@ -1403,7 +1478,9 @@
     <row r="57" spans="2:5" ht="30" customHeight="1">
       <c r="B57" s="11"/>
       <c r="C57" s="9"/>
-      <c r="D57" s="7"/>
+      <c r="D57" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E57" s="1" t="s">
         <v>72</v>
       </c>
@@ -1411,7 +1488,9 @@
     <row r="58" spans="2:5" ht="30" customHeight="1">
       <c r="B58" s="11"/>
       <c r="C58" s="9"/>
-      <c r="D58" s="7"/>
+      <c r="D58" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E58" s="1" t="s">
         <v>73</v>
       </c>
@@ -1421,7 +1500,9 @@
       <c r="C59" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D59" s="7"/>
+      <c r="D59" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E59" s="1" t="s">
         <v>75</v>
       </c>
@@ -1429,7 +1510,9 @@
     <row r="60" spans="2:5" ht="30" customHeight="1">
       <c r="B60" s="11"/>
       <c r="C60" s="9"/>
-      <c r="D60" s="7"/>
+      <c r="D60" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E60" s="1" t="s">
         <v>76</v>
       </c>
@@ -1439,7 +1522,9 @@
       <c r="C61" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D61" s="7"/>
+      <c r="D61" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E61" s="1" t="s">
         <v>78</v>
       </c>
@@ -1447,7 +1532,9 @@
     <row r="62" spans="2:5" ht="30" customHeight="1">
       <c r="B62" s="11"/>
       <c r="C62" s="9"/>
-      <c r="D62" s="7"/>
+      <c r="D62" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E62" s="1" t="s">
         <v>79</v>
       </c>
@@ -1457,7 +1544,9 @@
       <c r="C63" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D63" s="7"/>
+      <c r="D63" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E63" s="1" t="s">
         <v>81</v>
       </c>
@@ -1465,7 +1554,9 @@
     <row r="64" spans="2:5" ht="30" customHeight="1">
       <c r="B64" s="11"/>
       <c r="C64" s="9"/>
-      <c r="D64" s="7"/>
+      <c r="D64" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E64" s="1" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
I updated the rubric
</commit_message>
<xml_diff>
--- a/Rubric.xlsx
+++ b/Rubric.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattj13\Documents\GitHub\would-you-rather\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewrobertson/Documents/gitRepos/would-you-rather/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26760" windowHeight="10800"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="Checkboxes">Sheet1!$D$4:$D$5,Sheet1!$D$7:$D$11,Sheet1!$D$13:$D$53,Sheet1!$D$56:$D$64</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="86">
   <si>
     <t>CRITERIA</t>
   </si>
@@ -389,7 +389,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -577,45 +577,45 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,50 +906,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="51.42578125" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
-    <col min="5" max="5" width="117.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="51.5" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" customWidth="1"/>
+    <col min="5" max="5" width="117.5" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" customHeight="1">
-      <c r="B1" s="19" t="str">
+      <c r="B1" s="18" t="str">
         <f>"Due "&amp;TEXT(I4,"ddd, mmmm d")</f>
         <v>Due Thu, June 21</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21" t="str">
+      <c r="C1" s="19"/>
+      <c r="D1" s="16" t="str">
         <f ca="1">I5&amp;" DAYS REMAINING"</f>
-        <v>10 DAYS REMAINING</v>
-      </c>
-      <c r="E1" s="21"/>
+        <v>8 DAYS REMAINING</v>
+      </c>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="2:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="2:9">
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="15"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -959,13 +959,13 @@
       <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="14">
         <f>DATE(2018,6,21)</f>
         <v>43272</v>
       </c>
     </row>
     <row r="5" spans="2:9" s="6" customFormat="1" ht="30" customHeight="1">
-      <c r="B5" s="12"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
@@ -973,19 +973,19 @@
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="15">
         <f ca="1">DATEDIF(TODAY(), I4,"D")</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:9" s="6" customFormat="1" ht="12.75" customHeight="1" thickBot="1">
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="I6" s="18"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="2:9" ht="30" customHeight="1">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="21" t="s">
         <v>68</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -997,11 +997,11 @@
       <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="17"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="2:9" ht="30" customHeight="1">
-      <c r="B8" s="11"/>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="20" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1012,8 +1012,8 @@
       </c>
     </row>
     <row r="9" spans="2:9" ht="30" customHeight="1">
-      <c r="B9" s="11"/>
-      <c r="C9" s="9"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="3" t="s">
         <v>85</v>
       </c>
@@ -1022,8 +1022,8 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="30" customHeight="1">
-      <c r="B10" s="11"/>
-      <c r="C10" s="9"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="3" t="s">
         <v>85</v>
       </c>
@@ -1032,8 +1032,8 @@
       </c>
     </row>
     <row r="11" spans="2:9" ht="30" customHeight="1">
-      <c r="B11" s="11"/>
-      <c r="C11" s="9"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="3" t="s">
         <v>85</v>
       </c>
@@ -1042,10 +1042,10 @@
       </c>
     </row>
     <row r="13" spans="2:9" ht="30" customHeight="1">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="20" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1056,8 +1056,8 @@
       </c>
     </row>
     <row r="14" spans="2:9" ht="30" customHeight="1">
-      <c r="B14" s="11"/>
-      <c r="C14" s="9"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="7" t="s">
         <v>85</v>
       </c>
@@ -1066,8 +1066,8 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="30" customHeight="1">
-      <c r="B15" s="11"/>
-      <c r="C15" s="9"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="7" t="s">
         <v>85</v>
       </c>
@@ -1076,8 +1076,8 @@
       </c>
     </row>
     <row r="16" spans="2:9" ht="30" customHeight="1">
-      <c r="B16" s="11"/>
-      <c r="C16" s="9"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="7" t="s">
         <v>85</v>
       </c>
@@ -1086,20 +1086,20 @@
       </c>
     </row>
     <row r="17" spans="2:19" ht="30" customHeight="1">
-      <c r="B17" s="11"/>
-      <c r="C17" s="9"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="7" t="s">
         <v>85</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
     </row>
     <row r="18" spans="2:19" ht="30" customHeight="1">
-      <c r="B18" s="11"/>
-      <c r="C18" s="9"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="7" t="s">
         <v>85</v>
       </c>
@@ -1108,8 +1108,8 @@
       </c>
     </row>
     <row r="19" spans="2:19" ht="30" customHeight="1">
-      <c r="B19" s="11"/>
-      <c r="C19" s="9" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="7" t="s">
@@ -1120,8 +1120,8 @@
       </c>
     </row>
     <row r="20" spans="2:19" ht="30" customHeight="1">
-      <c r="B20" s="11"/>
-      <c r="C20" s="9"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="7" t="s">
         <v>85</v>
       </c>
@@ -1130,8 +1130,8 @@
       </c>
     </row>
     <row r="21" spans="2:19" ht="30" customHeight="1">
-      <c r="B21" s="11"/>
-      <c r="C21" s="9"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="7" t="s">
         <v>85</v>
       </c>
@@ -1140,10 +1140,10 @@
       </c>
     </row>
     <row r="22" spans="2:19" ht="30" customHeight="1">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="20" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="7" t="s">
@@ -1154,44 +1154,48 @@
       </c>
     </row>
     <row r="23" spans="2:19" ht="30" customHeight="1">
-      <c r="B23" s="11"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="7"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E23" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:19" ht="30" customHeight="1">
-      <c r="B24" s="11"/>
-      <c r="C24" s="9"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:19" ht="30" customHeight="1">
-      <c r="B25" s="11"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="10" t="s">
+      <c r="B25" s="21"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="2:19" ht="30" customHeight="1">
-      <c r="B26" s="11"/>
-      <c r="C26" s="9"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="27" spans="2:19" ht="30" customHeight="1">
-      <c r="B27" s="11"/>
-      <c r="C27" s="9"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="7" t="s">
         <v>85</v>
       </c>
@@ -1200,38 +1204,38 @@
       </c>
     </row>
     <row r="28" spans="2:19" ht="30" customHeight="1">
-      <c r="B28" s="11"/>
-      <c r="C28" s="9"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="20"/>
       <c r="D28" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="29" spans="2:19" ht="30" customHeight="1">
-      <c r="B29" s="11"/>
-      <c r="C29" s="9"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:19" ht="30" customHeight="1">
-      <c r="B30" s="11"/>
-      <c r="C30" s="9"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="31" spans="2:19" ht="30" customHeight="1">
-      <c r="B31" s="11"/>
-      <c r="C31" s="9"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="7" t="s">
         <v>85</v>
       </c>
@@ -1240,8 +1244,8 @@
       </c>
     </row>
     <row r="32" spans="2:19" ht="30" customHeight="1">
-      <c r="B32" s="11"/>
-      <c r="C32" s="9"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="7" t="s">
         <v>85</v>
       </c>
@@ -1250,8 +1254,8 @@
       </c>
     </row>
     <row r="33" spans="2:5" ht="30" customHeight="1">
-      <c r="B33" s="11"/>
-      <c r="C33" s="9"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="20"/>
       <c r="D33" s="7" t="s">
         <v>85</v>
       </c>
@@ -1260,8 +1264,8 @@
       </c>
     </row>
     <row r="34" spans="2:5" ht="30" customHeight="1">
-      <c r="B34" s="11"/>
-      <c r="C34" s="9" t="s">
+      <c r="B34" s="21"/>
+      <c r="C34" s="20" t="s">
         <v>37</v>
       </c>
       <c r="D34" s="7" t="s">
@@ -1272,8 +1276,8 @@
       </c>
     </row>
     <row r="35" spans="2:5" ht="30" customHeight="1">
-      <c r="B35" s="11"/>
-      <c r="C35" s="9"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="20"/>
       <c r="D35" s="7" t="s">
         <v>85</v>
       </c>
@@ -1282,8 +1286,8 @@
       </c>
     </row>
     <row r="36" spans="2:5" ht="30" customHeight="1">
-      <c r="B36" s="11"/>
-      <c r="C36" s="9"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="20"/>
       <c r="D36" s="7" t="s">
         <v>85</v>
       </c>
@@ -1292,18 +1296,18 @@
       </c>
     </row>
     <row r="37" spans="2:5" ht="30" customHeight="1">
-      <c r="B37" s="11"/>
-      <c r="C37" s="9"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="7"/>
       <c r="E37" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="30" customHeight="1">
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="20" t="s">
         <v>42</v>
       </c>
       <c r="D38" s="7" t="s">
@@ -1314,8 +1318,8 @@
       </c>
     </row>
     <row r="39" spans="2:5" ht="30" customHeight="1">
-      <c r="B39" s="11"/>
-      <c r="C39" s="9"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="20"/>
       <c r="D39" s="7" t="s">
         <v>85</v>
       </c>
@@ -1324,16 +1328,18 @@
       </c>
     </row>
     <row r="40" spans="2:5" ht="30" customHeight="1">
-      <c r="B40" s="11"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="7"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="E40" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="30" customHeight="1">
-      <c r="B41" s="11"/>
-      <c r="C41" s="9"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="20"/>
       <c r="D41" s="7" t="s">
         <v>85</v>
       </c>
@@ -1342,10 +1348,10 @@
       </c>
     </row>
     <row r="42" spans="2:5" ht="30" customHeight="1">
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="20" t="s">
         <v>47</v>
       </c>
       <c r="D42" s="7" t="s">
@@ -1356,58 +1362,58 @@
       </c>
     </row>
     <row r="43" spans="2:5" ht="30" customHeight="1">
-      <c r="B43" s="11"/>
-      <c r="C43" s="9"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="20"/>
       <c r="D43" s="7"/>
       <c r="E43" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="30" customHeight="1">
-      <c r="B44" s="11"/>
-      <c r="C44" s="9"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="20"/>
       <c r="D44" s="7"/>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="30" customHeight="1">
-      <c r="B45" s="11"/>
-      <c r="C45" s="9"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="20"/>
       <c r="D45" s="7"/>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="30" customHeight="1">
-      <c r="B46" s="11"/>
-      <c r="C46" s="9"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="20"/>
       <c r="D46" s="7"/>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="9" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="30" customHeight="1">
-      <c r="B47" s="11"/>
-      <c r="C47" s="9"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="20"/>
       <c r="D47" s="7"/>
-      <c r="E47" s="10" t="s">
+      <c r="E47" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="48" spans="2:5" ht="30" customHeight="1">
-      <c r="B48" s="11"/>
-      <c r="C48" s="9"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="20"/>
       <c r="D48" s="7"/>
       <c r="E48" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="30" customHeight="1">
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="20" t="s">
         <v>55</v>
       </c>
       <c r="D49" s="7" t="s">
@@ -1418,8 +1424,8 @@
       </c>
     </row>
     <row r="50" spans="2:5" ht="30" customHeight="1">
-      <c r="B50" s="11"/>
-      <c r="C50" s="9"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="20"/>
       <c r="D50" s="7" t="s">
         <v>85</v>
       </c>
@@ -1428,10 +1434,10 @@
       </c>
     </row>
     <row r="51" spans="2:5" ht="30" customHeight="1">
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="20" t="s">
         <v>58</v>
       </c>
       <c r="D51" s="7" t="s">
@@ -1442,8 +1448,8 @@
       </c>
     </row>
     <row r="52" spans="2:5" ht="30" customHeight="1">
-      <c r="B52" s="11"/>
-      <c r="C52" s="9"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="20"/>
       <c r="D52" s="7" t="s">
         <v>85</v>
       </c>
@@ -1462,10 +1468,10 @@
       </c>
     </row>
     <row r="56" spans="2:5" ht="30" customHeight="1">
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C56" s="20" t="s">
         <v>70</v>
       </c>
       <c r="D56" s="7" t="s">
@@ -1476,8 +1482,8 @@
       </c>
     </row>
     <row r="57" spans="2:5" ht="30" customHeight="1">
-      <c r="B57" s="11"/>
-      <c r="C57" s="9"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="20"/>
       <c r="D57" s="7" t="s">
         <v>85</v>
       </c>
@@ -1486,8 +1492,8 @@
       </c>
     </row>
     <row r="58" spans="2:5" ht="30" customHeight="1">
-      <c r="B58" s="11"/>
-      <c r="C58" s="9"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="20"/>
       <c r="D58" s="7" t="s">
         <v>85</v>
       </c>
@@ -1496,8 +1502,8 @@
       </c>
     </row>
     <row r="59" spans="2:5" ht="30" customHeight="1">
-      <c r="B59" s="11"/>
-      <c r="C59" s="9" t="s">
+      <c r="B59" s="21"/>
+      <c r="C59" s="20" t="s">
         <v>74</v>
       </c>
       <c r="D59" s="7" t="s">
@@ -1508,8 +1514,8 @@
       </c>
     </row>
     <row r="60" spans="2:5" ht="30" customHeight="1">
-      <c r="B60" s="11"/>
-      <c r="C60" s="9"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="20"/>
       <c r="D60" s="7" t="s">
         <v>85</v>
       </c>
@@ -1518,8 +1524,8 @@
       </c>
     </row>
     <row r="61" spans="2:5" ht="30" customHeight="1">
-      <c r="B61" s="11"/>
-      <c r="C61" s="9" t="s">
+      <c r="B61" s="21"/>
+      <c r="C61" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D61" s="7" t="s">
@@ -1530,8 +1536,8 @@
       </c>
     </row>
     <row r="62" spans="2:5" ht="30" customHeight="1">
-      <c r="B62" s="11"/>
-      <c r="C62" s="9"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="20"/>
       <c r="D62" s="7" t="s">
         <v>85</v>
       </c>
@@ -1540,8 +1546,8 @@
       </c>
     </row>
     <row r="63" spans="2:5" ht="30" customHeight="1">
-      <c r="B63" s="11"/>
-      <c r="C63" s="9" t="s">
+      <c r="B63" s="21"/>
+      <c r="C63" s="20" t="s">
         <v>80</v>
       </c>
       <c r="D63" s="7" t="s">
@@ -1552,8 +1558,8 @@
       </c>
     </row>
     <row r="64" spans="2:5" ht="30" customHeight="1">
-      <c r="B64" s="11"/>
-      <c r="C64" s="9"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="20"/>
       <c r="D64" s="7" t="s">
         <v>85</v>
       </c>
@@ -1563,11 +1569,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C61:C62"/>
     <mergeCell ref="C63:C64"/>
     <mergeCell ref="B56:B64"/>
     <mergeCell ref="D3:E3"/>
@@ -1584,6 +1585,11 @@
     <mergeCell ref="C38:C41"/>
     <mergeCell ref="C42:C48"/>
     <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C61:C62"/>
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="C13:C18"/>

</xml_diff>